<commit_message>
Redoing experiment 2 collecting more measures
</commit_message>
<xml_diff>
--- a/results_2.xlsx
+++ b/results_2.xlsx
@@ -20,14 +20,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="119">
   <si>
     <t xml:space="preserve">PLS</t>
   </si>
   <si>
-    <t xml:space="preserve">P1_P3</t>
-  </si>
-  <si>
     <t xml:space="preserve">m</t>
   </si>
   <si>
@@ -61,6 +58,9 @@
     <t xml:space="preserve">Computational_Time(s)</t>
   </si>
   <si>
+    <t xml:space="preserve">Memory_Used(MiB)</t>
+  </si>
+  <si>
     <t xml:space="preserve">50</t>
   </si>
   <si>
@@ -70,43 +70,49 @@
     <t xml:space="preserve">12</t>
   </si>
   <si>
-    <t xml:space="preserve">32.26438949919196</t>
+    <t xml:space="preserve">32.481781117399834</t>
   </si>
   <si>
     <t xml:space="preserve">600.0</t>
   </si>
   <si>
-    <t xml:space="preserve">6.074890280510293e-14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.8395938583379771</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.463600183287116e-14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5.2891237786088754e-14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.1868693828582764</t>
-  </si>
-  <si>
-    <t xml:space="preserve">32.26438949918736</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.0841563659039797e-12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.8395938583399148</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.724115538872147e-11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.475595224082124e-10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8.01587200164795</t>
+    <t xml:space="preserve">2.901587644069545e-14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.8548963495952719</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.5585729564121144e-14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.955663653437544e-14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16.75049114227295</t>
+  </si>
+  <si>
+    <t xml:space="preserve">76.06452560424805</t>
+  </si>
+  <si>
+    <t xml:space="preserve">32.48178111739868</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.9165194962834017e-12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.8548963495952443</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.368431381506578e-12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.0929424124180145e-11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26.308172702789307</t>
+  </si>
+  <si>
+    <t xml:space="preserve">85.16492557525635</t>
   </si>
   <si>
     <t xml:space="preserve">60</t>
@@ -118,43 +124,49 @@
     <t xml:space="preserve">15</t>
   </si>
   <si>
-    <t xml:space="preserve">40.67689166903868</t>
+    <t xml:space="preserve">40.80398931130086</t>
   </si>
   <si>
     <t xml:space="preserve">900.0</t>
   </si>
   <si>
-    <t xml:space="preserve">6.143992304383014e-14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.8433581519974804</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.6799182182858837e-14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5.69579101545366e-14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.175321102142334</t>
-  </si>
-  <si>
-    <t xml:space="preserve">40.67689166903894</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8.609483502135014e-13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.8433581519975532</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8.881156707897367e-13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4.064320011715042e-12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">43.48126792907715</t>
+    <t xml:space="preserve">7.302945613073911e-14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.8705569304598669</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.283703900104093e-14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7.145414806947204e-14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">31.366809129714966</t>
+  </si>
+  <si>
+    <t xml:space="preserve">165.6187505722046</t>
+  </si>
+  <si>
+    <t xml:space="preserve">40.80398931132339</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.3284933971556331e-11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.8705569304605574</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.0369248095667723e-11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.5042003191671894e-11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">67.99174809455872</t>
+  </si>
+  <si>
+    <t xml:space="preserve">176.90629386901855</t>
   </si>
   <si>
     <t xml:space="preserve">70</t>
@@ -166,43 +178,49 @@
     <t xml:space="preserve">17</t>
   </si>
   <si>
-    <t xml:space="preserve">46.26152517197252</t>
+    <t xml:space="preserve">46.41084843039981</t>
   </si>
   <si>
     <t xml:space="preserve">1190.0</t>
   </si>
   <si>
-    <t xml:space="preserve">1.207489394514566e-13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.8387192876184119</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.476334503768754e-14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7.875653022878451e-14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.8211429119110107</t>
-  </si>
-  <si>
-    <t xml:space="preserve">46.26152517195999</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.1793062849006057e-11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.8387192876177038</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.5683801543444264e-11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.0576134626708322e-10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">89.2492048740387</t>
+    <t xml:space="preserve">9.719172322860145e-14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.8710959375676282</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.2651783806525894e-14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9.57293274197283e-14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">55.28808832168579</t>
+  </si>
+  <si>
+    <t xml:space="preserve">297.4272184371948</t>
+  </si>
+  <si>
+    <t xml:space="preserve">46.41084843026661</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.286210153154025e-10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.8710959375651665</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7.852769857497326e-11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.6481947322422525e-10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">146.43056058883667</t>
+  </si>
+  <si>
+    <t xml:space="preserve">323.7890100479126</t>
   </si>
   <si>
     <t xml:space="preserve">80</t>
@@ -214,43 +232,49 @@
     <t xml:space="preserve">20</t>
   </si>
   <si>
-    <t xml:space="preserve">54.82510747728131</t>
+    <t xml:space="preserve">55.56381306091273</t>
   </si>
   <si>
     <t xml:space="preserve">1600.0</t>
   </si>
   <si>
-    <t xml:space="preserve">2.568170905575366e-12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.874354650146805</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.1130075351690318e-12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.56835072656505e-12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5.907901287078857</t>
-  </si>
-  <si>
-    <t xml:space="preserve">54.825107477277186</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.793030179002634e-12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.8743546501466474</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.8763799599698672e-12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.817223137438521e-11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">199.93035435676575</t>
+    <t xml:space="preserve">1.1947176084732957e-13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.8883422032267924</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5.655271498066419e-14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.3013228866980505e-13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">88.98524475097656</t>
+  </si>
+  <si>
+    <t xml:space="preserve">500.89677143096924</t>
+  </si>
+  <si>
+    <t xml:space="preserve">55.56381306098904</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.680472965531312e-11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.8883422032271318</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.7754025016908623e-11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.1302671471522354e-10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">298.79980850219727</t>
+  </si>
+  <si>
+    <t xml:space="preserve">534.0571479797363</t>
   </si>
   <si>
     <t xml:space="preserve">90</t>
@@ -262,85 +286,97 @@
     <t xml:space="preserve">22</t>
   </si>
   <si>
-    <t xml:space="preserve">60.823281594090545</t>
+    <t xml:space="preserve">60.51276199998328</t>
   </si>
   <si>
     <t xml:space="preserve">1980.0</t>
   </si>
   <si>
-    <t xml:space="preserve">2.2179673984717947e-13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.8941361852261699</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7.683794331338956e-14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.8786499539255812e-13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9.459279537200928</t>
-  </si>
-  <si>
-    <t xml:space="preserve">60.82328159409139</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.40683023953836e-11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.8941361852254919</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.6008685238862947e-11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9.008335043457373e-11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">343.7252597808838</t>
+    <t xml:space="preserve">1.7294592590195796e-12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.899504552596678</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6.703791803419323e-13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.53802779773062e-12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">135.5402910709381</t>
+  </si>
+  <si>
+    <t xml:space="preserve">794.1871404647827</t>
+  </si>
+  <si>
+    <t xml:space="preserve">60.512762651993</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.035396739439763e-12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.8995045456257088</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.5860727351816737e-12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.7667540323380115e-11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">460.86738419532776</t>
+  </si>
+  <si>
+    <t xml:space="preserve">837.5782518386841</t>
   </si>
   <si>
     <t xml:space="preserve">100</t>
   </si>
   <si>
-    <t xml:space="preserve">70.05086579165344</t>
+    <t xml:space="preserve">69.46632606281258</t>
   </si>
   <si>
     <t xml:space="preserve">2500.0</t>
   </si>
   <si>
-    <t xml:space="preserve">3.8731178962525147e-13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.9116740901727752</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.3131914476033657e-13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.139568024495029e-13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13.880299091339111</t>
-  </si>
-  <si>
-    <t xml:space="preserve">70.05086579165626</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.4703252956642633e-12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.9116740901743073</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5.824135156992599e-11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.88649832959585e-10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">775.304249048233</t>
+    <t xml:space="preserve">3.655902068524086e-12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.9006748242100917</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.4052423803959695e-12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.184460159366351e-12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">194.80895948410034</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1188.3532094955444</t>
+  </si>
+  <si>
+    <t xml:space="preserve">69.46632606279377</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.6917187067307912e-11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.9006748242093315</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9.27907909518647e-12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6.578148863103145e-11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">883.6329827308655</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1246.5071077346802</t>
   </si>
 </sst>
 </file>
@@ -444,7 +480,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -712,26 +748,27 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S8"/>
+  <dimension ref="A1:U8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O12" activeCellId="0" sqref="O12"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="24.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="21.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="0" width="24.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="21.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="21.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="8.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="24.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="21.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="17" style="0" width="24.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="21.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="19.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="8.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="24.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="21.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="18" style="0" width="24.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="21.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="21.04"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -745,9 +782,7 @@
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
-      <c r="L1" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="L1" s="1"/>
       <c r="M1" s="2"/>
       <c r="N1" s="2"/>
       <c r="O1" s="2"/>
@@ -755,63 +790,71 @@
       <c r="Q1" s="2"/>
       <c r="R1" s="2"/>
       <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="I2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="J2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="K2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="L2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="M2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="N2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="O2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="P2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="O2" s="5" t="s">
+      <c r="Q2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="P2" s="5" t="s">
+      <c r="R2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="Q2" s="5" t="s">
+      <c r="S2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="R2" s="5" t="s">
+      <c r="T2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="S2" s="5" t="s">
+      <c r="U2" s="5" t="s">
         <v>12</v>
       </c>
     </row>
@@ -853,13 +896,13 @@
         <v>23</v>
       </c>
       <c r="M3" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="N3" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="N3" s="0" t="s">
+      <c r="O3" s="0" t="s">
         <v>14</v>
-      </c>
-      <c r="O3" s="0" t="s">
-        <v>24</v>
       </c>
       <c r="P3" s="0" t="s">
         <v>25</v>
@@ -872,247 +915,277 @@
       </c>
       <c r="S3" s="0" t="s">
         <v>28</v>
+      </c>
+      <c r="T3" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="U3" s="0" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D4" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="F4" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="E4" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="F4" s="0" t="s">
-        <v>30</v>
-      </c>
       <c r="G4" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="H4" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="J4" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="K4" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="L4" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="M4" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="N4" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="I4" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="J4" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="K4" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="L4" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="M4" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="N4" s="0" t="s">
-        <v>30</v>
-      </c>
       <c r="O4" s="0" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="P4" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="Q4" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="R4" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="S4" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
+      </c>
+      <c r="T4" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="U4" s="0" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="G5" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="I5" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="J5" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="K5" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="L5" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="M5" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="N5" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="O5" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="H5" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="I5" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="J5" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="K5" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="L5" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="M5" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="N5" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="O5" s="0" t="s">
-        <v>56</v>
-      </c>
       <c r="P5" s="0" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="Q5" s="0" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="R5" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="S5" s="0" t="s">
-        <v>60</v>
+        <v>64</v>
+      </c>
+      <c r="T5" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="U5" s="0" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="I6" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="J6" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="K6" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="L6" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="M6" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="N6" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="O6" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="J6" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="K6" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="L6" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="M6" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="N6" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="O6" s="0" t="s">
-        <v>72</v>
-      </c>
       <c r="P6" s="0" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="Q6" s="0" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="R6" s="0" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="S6" s="0" t="s">
-        <v>76</v>
+        <v>82</v>
+      </c>
+      <c r="T6" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="U6" s="0" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="J7" s="0" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="K7" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="L7" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="M7" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="N7" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="O7" s="0" t="s">
         <v>86</v>
       </c>
-      <c r="L7" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="M7" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="N7" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="O7" s="0" t="s">
-        <v>88</v>
-      </c>
       <c r="P7" s="0" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="Q7" s="0" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="R7" s="0" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="S7" s="0" t="s">
-        <v>92</v>
+        <v>100</v>
+      </c>
+      <c r="T7" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="U7" s="0" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="B8" s="0" t="s">
         <v>13</v>
@@ -1121,52 +1194,58 @@
         <v>14</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="F8" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="J8" s="0" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
       <c r="K8" s="0" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="L8" s="0" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="M8" s="0" t="s">
-        <v>95</v>
+        <v>112</v>
       </c>
       <c r="N8" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="O8" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="O8" s="0" t="s">
-        <v>102</v>
-      </c>
       <c r="P8" s="0" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="Q8" s="0" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
       <c r="R8" s="0" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="S8" s="0" t="s">
-        <v>106</v>
+        <v>116</v>
+      </c>
+      <c r="T8" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="U8" s="0" t="s">
+        <v>118</v>
       </c>
     </row>
   </sheetData>

</xml_diff>